<commit_message>
v1.1 checking the reviews and changing their status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938DF48-077F-4493-9D29-F7F89976D6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="LH-TC-SYSTEMCONSTRAINS-REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>Author</t>
   </si>
@@ -175,12 +165,24 @@
   </si>
   <si>
     <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_005</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>NotApplicable</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Check reviews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,12 +682,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
       <calculatedColumnFormula>DATE(2025,4,22)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -694,18 +696,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1007,11 +1009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,10 +1053,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45769</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1071,11 +1081,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1151,7 +1161,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>17</v>
@@ -1183,7 +1193,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>17</v>
@@ -1215,7 +1225,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>17</v>
@@ -1247,7 +1257,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>17</v>
@@ -1279,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>17</v>
@@ -1311,7 +1321,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>17</v>
@@ -1343,7 +1353,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>17</v>
@@ -1388,13 +1398,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.2 All reviewer verifications have been closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938DF48-077F-4493-9D29-F7F89976D6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="LH-TC-SYSTEMCONSTRAINS-REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Author</t>
   </si>
@@ -77,9 +76,6 @@
   </si>
   <si>
     <t>Hala Eldaly</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Gehad Ashry</t>
@@ -177,12 +173,18 @@
   </si>
   <si>
     <t>Check reviews</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>All reviewer verifications have been closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,12 +684,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
+    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" name="Date" dataDxfId="12">
       <calculatedColumnFormula>DATE(2025,4,22)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -696,18 +698,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="9"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1009,18 +1011,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1054,23 +1056,31 @@
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="4">
         <v>45769</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45771</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1081,11 +1091,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1143,7 +1153,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>16</v>
@@ -1152,19 +1162,19 @@
         <v>2</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.35">
@@ -1172,10 +1182,10 @@
         <v>45769</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
@@ -1184,19 +1194,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="210" x14ac:dyDescent="0.35">
@@ -1204,10 +1214,10 @@
         <v>45769</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>16</v>
@@ -1216,19 +1226,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.35">
@@ -1236,10 +1246,10 @@
         <v>45769</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>16</v>
@@ -1248,19 +1258,19 @@
         <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1268,10 +1278,10 @@
         <v>45769</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>16</v>
@@ -1280,19 +1290,19 @@
         <v>2</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="H6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.35">
@@ -1300,10 +1310,10 @@
         <v>45769</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>16</v>
@@ -1312,19 +1322,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.35">
@@ -1332,10 +1342,10 @@
         <v>45769</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>16</v>
@@ -1344,19 +1354,19 @@
         <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="H8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1398,13 +1408,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v2.0 reviewed testcases for sys-contraints according to new srs
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\Group-3-Learning-hub-dev (1)\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD8D25-7192-4596-A364-E2AD12BD0D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name="LH-TC-SYSTEMCONSTRAINS-REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Author</t>
   </si>
@@ -72,9 +84,6 @@
     <t>Reviewed Entity</t>
   </si>
   <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_001</t>
-  </si>
-  <si>
     <t>Hala Eldaly</t>
   </si>
   <si>
@@ -87,24 +96,12 @@
     <t xml:space="preserve">File Template </t>
   </si>
   <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_002</t>
-  </si>
-  <si>
     <t xml:space="preserve">The test case sheet tab is not named according to the standard naming convention. </t>
   </si>
   <si>
     <t xml:space="preserve">Rename the sheet tab to "LH_TC_SYSTEMCONSTRAINTS" to match the correct format. </t>
   </si>
   <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_003</t>
-  </si>
-  <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_004</t>
-  </si>
-  <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_006</t>
-  </si>
-  <si>
     <t xml:space="preserve">LH-TC-SYSTEMCONSTRAINT-001 </t>
   </si>
   <si>
@@ -112,9 +109,6 @@
   </si>
   <si>
     <t>LH-TC-SYSTEMCONSTRAINT-004</t>
-  </si>
-  <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_007</t>
   </si>
   <si>
     <t xml:space="preserve">All test case IDs contain a typo in the word "SYSTEMCONSTRAINT" — the trailing "S" is missing. </t>
@@ -160,9 +154,6 @@
 </t>
   </si>
   <si>
-    <t>LH_TC_SYSTEMCONSTRAINTS_REVIEW_005</t>
-  </si>
-  <si>
     <t>Closed</t>
   </si>
   <si>
@@ -179,12 +170,59 @@
   </si>
   <si>
     <t>All reviewer verifications have been closed</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>Reviewed and closed thre reviews on v2.0</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_008</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_001</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_002</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_003</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_004</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_005</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_006</t>
+  </si>
+  <si>
+    <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_007</t>
+  </si>
+  <si>
+    <t>LH-TC-SYSTEMCONSTRAINTS-003
+LH-TC-SYSTEMCONSTRAINTS-004
+LH-TC-SYSTEMCONSTRAINTS-005</t>
+  </si>
+  <si>
+    <t>where to check for the user id</t>
+  </si>
+  <si>
+    <t>add details on  where to check for the user id after registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -267,6 +305,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +696,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -684,12 +728,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
       <calculatedColumnFormula>DATE(2025,4,22)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -698,18 +742,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1011,22 +1055,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1040,12 +1084,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1054,32 +1098,47 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4">
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4">
         <v>45771</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="10">
+        <f>DATE(2025,5,11)</f>
+        <v>45788</v>
       </c>
     </row>
   </sheetData>
@@ -1091,29 +1150,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="84.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="88.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="18.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="56.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="84.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="88.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1145,243 +1204,264 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
         <v>45769</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A3" s="8">
         <v>45769</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="210" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="210" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>45769</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>45</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <v>45769</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>45769</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>45769</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A8" s="8">
         <v>45769</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+      <c r="A9" s="11">
+        <f>DATE(2025,5,11)</f>
+        <v>45788</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="E9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="I9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1393,7 +1473,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1408,13 +1488,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v2.1 closed the review comments on v2.0
LH_TC_SYSTEMCONSTRAINS_REVIEW
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_SYSTEMCONSTRAINTS_REVIEWS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\Group-3-Learning-hub-dev (1)\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD8D25-7192-4596-A364-E2AD12BD0D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879BA4A1-F492-4FDD-845E-EC7AFB372DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>Author</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Mahmoud Abdelmageed</t>
-  </si>
-  <si>
-    <t>Reviewed and closed thre reviews on v2.0</t>
   </si>
   <si>
     <t>LH-REVIEW-TC-SYSTEMCONSTRAINTS-REVIEW_008</t>
@@ -214,6 +211,15 @@
   </si>
   <si>
     <t>add details on  where to check for the user id after registration</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>Reviewed on v2.0 according to new srs</t>
+  </si>
+  <si>
+    <t>closed the reviews on v2.0</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
@@ -802,7 +808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -854,7 +860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1056,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,14 +1140,30 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D5" s="10">
         <f>DATE(2025,5,11)</f>
         <v>45788</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="10">
+        <f>DATE(2025,5,11)</f>
+        <v>45788</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1153,7 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1166,7 +1188,7 @@
     <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="84.33203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="88.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="5" customWidth="1"/>
     <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
     <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="5"/>
@@ -1209,7 +1231,7 @@
         <v>45769</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -1241,7 +1263,7 @@
         <v>45769</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>30</v>
@@ -1268,12 +1290,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="210" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="189" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>45769</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>21</v>
@@ -1305,7 +1327,7 @@
         <v>45769</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>22</v>
@@ -1337,7 +1359,7 @@
         <v>45769</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>23</v>
@@ -1369,7 +1391,7 @@
         <v>45769</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>31</v>
@@ -1401,7 +1423,7 @@
         <v>45769</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>28</v>
@@ -1434,10 +1456,10 @@
         <v>45788</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>45</v>
@@ -1446,10 +1468,10 @@
         <v>44</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>45</v>

</xml_diff>